<commit_message>
No Evap Plots R Update
Created Plots for Data with No Evap
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/Outputs/OutputAnnualDemandsRiverSMART.xlsx
+++ b/2 - RiverWare Modeling/Outputs/OutputAnnualDemandsRiverSMART.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7666" uniqueCount="22">
   <si>
     <t>Demand Data.AnnualDemands</t>
   </si>
@@ -121,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1083">
+  <borders count="2672">
     <border>
       <left/>
       <right/>
@@ -1235,11 +1235,1600 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1085">
+  <cellXfs count="2674">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -2639,6 +4228,2049 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1080" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1081" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1082" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1083" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1084" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1085" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1086" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1087" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1088" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1089" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1090" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1091" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1092" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1093" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1094" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1095" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1096" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1097" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1098" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1099" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1103" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1110" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1117" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1124" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1131" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1138" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1145" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1152" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1159" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1166" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1173" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1180" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1187" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1194" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1201" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1208" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1215" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1222" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1229" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1236" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1243" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1250" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1257" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1264" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1271" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1278" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1285" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1292" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1299" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1306" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1313" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1320" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1327" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1334" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1341" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1348" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1355" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1362" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1369" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1376" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1383" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1390" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1397" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1404" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1411" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1418" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1425" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1432" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1439" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1446" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1453" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1460" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1467" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1474" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1481" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1483" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1488" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1490" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1495" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1497" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1502" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1504" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1509" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1510" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1511" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1516" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1517" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1518" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1523" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1524" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1525" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1530" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1537" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1538" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1544" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1551" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1558" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1565" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1567" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1572" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1573" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1574" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1579" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1580" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1581" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1586" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1587" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1588" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1593" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1594" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1595" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1600" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1601" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1602" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1607" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1608" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1609" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1614" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1621" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1628" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1635" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1636" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1637" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1642" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1643" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1644" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1649" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1650" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1651" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1656" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1657" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1658" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1663" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1664" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1665" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1670" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1672" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1677" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1679" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1681" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1682" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1683" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1684" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1685" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1686" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1687" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1688" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1689" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1690" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1691" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1692" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1693" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1694" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1695" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1696" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1697" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1698" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1699" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1700" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1701" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1702" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1703" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1704" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1705" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1706" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1707" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1708" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1709" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1710" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1711" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1712" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1713" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1714" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1715" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1716" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1717" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1718" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1719" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1720" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1721" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1722" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1723" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1724" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1725" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1726" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1727" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1728" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1729" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1730" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1731" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1732" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1733" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1734" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1735" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1736" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1737" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1738" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1739" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1740" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1741" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1742" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1743" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1744" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1745" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1746" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1747" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1748" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1749" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1750" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1751" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1752" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1753" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1754" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1755" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1756" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1757" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1758" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1759" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1760" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1761" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1762" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1763" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1764" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1765" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1766" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1767" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1768" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1769" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1770" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1771" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1772" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1773" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1774" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1775" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1776" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1777" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1778" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1779" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1780" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1781" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1782" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1783" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1784" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1785" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1786" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1787" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1788" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1789" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1790" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1791" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1792" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1793" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1794" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1795" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1796" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1797" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1798" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1799" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1800" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1801" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1802" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1803" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1804" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1805" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1806" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1807" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1808" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1809" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1810" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1811" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1812" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1813" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1814" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1815" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1816" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1817" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1818" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1819" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1820" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1821" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1822" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1823" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1824" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1825" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1826" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1827" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1828" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1829" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1830" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1831" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1832" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1833" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1834" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1835" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1836" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1837" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1838" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1839" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1840" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1841" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1842" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1843" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1844" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1845" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1846" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1847" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1848" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1849" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1850" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1851" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1852" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1853" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1854" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1855" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1856" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1857" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1858" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1859" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1860" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1861" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1862" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1863" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1864" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1865" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1866" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1867" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1868" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1869" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1870" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1871" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1872" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1873" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1874" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1875" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1876" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1877" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1878" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1879" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1880" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1881" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1882" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1883" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1884" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1885" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1886" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1887" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1888" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1889" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1890" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1891" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1892" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1893" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1894" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1895" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1896" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1897" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1898" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1899" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1900" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1901" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1902" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1903" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1904" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1905" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1906" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1907" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1908" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1909" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1910" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1911" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1912" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1913" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1914" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1915" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1916" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1917" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1918" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1919" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1920" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1921" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1922" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1923" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1924" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1925" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1926" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1927" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1928" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1929" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1930" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1931" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1932" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1933" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1934" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1935" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1936" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1937" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1938" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1939" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1940" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1941" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1942" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1943" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1944" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1945" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1946" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1947" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1948" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1949" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1950" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1951" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1952" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1953" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1954" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1955" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1956" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1957" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1958" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1959" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1960" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1961" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1962" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1963" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1964" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1965" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1966" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1967" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1968" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1969" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1970" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1971" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1972" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1973" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1974" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1975" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1976" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1977" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1978" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1979" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1980" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1981" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1982" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1983" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1984" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1985" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1986" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1987" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1988" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1989" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1990" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1991" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1992" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1993" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1994" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1995" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1996" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1997" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1998" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1999" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2000" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2001" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2002" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2003" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2004" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2005" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2006" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2007" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2008" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2009" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2010" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2011" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2012" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2013" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2014" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2015" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2016" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2017" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2018" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2019" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2020" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2021" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2022" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2023" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2024" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2025" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2026" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2027" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2028" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2029" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2030" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2031" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2032" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2033" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2034" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2035" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2036" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2037" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2038" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2039" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2040" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2041" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2042" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2043" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2044" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2045" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2046" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2047" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2048" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2049" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2050" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2051" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2052" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2053" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2054" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2055" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2056" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2057" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2058" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2059" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2060" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2061" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2062" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2063" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2064" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2065" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2066" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2067" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2068" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2069" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2070" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2071" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2072" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2073" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2074" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2075" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2076" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2077" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2078" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2079" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2080" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2081" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2082" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2083" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2084" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2085" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2086" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2087" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2088" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2089" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2090" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2091" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2092" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2093" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2094" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2095" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2096" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2097" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2098" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2099" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2104" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2111" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2118" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2125" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2132" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2139" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2146" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2153" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2160" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2167" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2174" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2181" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2188" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2195" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2202" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2209" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2216" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2223" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2230" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2237" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2244" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2251" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2258" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2265" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2272" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2279" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2286" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2293" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2300" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2307" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2314" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2321" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2328" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2335" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2342" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2349" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2356" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2363" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2370" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2377" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2384" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2391" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2398" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2405" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2412" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2419" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2426" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2433" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2440" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2447" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2454" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2461" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2468" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2475" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2482" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2483" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2489" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2490" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2496" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2497" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2503" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2504" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2509" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2510" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2511" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2516" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2517" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2518" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2523" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2524" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2525" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2531" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2537" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2538" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2545" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2552" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2559" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2566" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2567" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2572" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2573" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2574" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2579" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2580" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2581" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2586" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2587" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2588" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2593" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2594" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2595" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2600" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2601" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2602" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2607" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2608" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2609" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2614" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2615" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2622" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2629" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2635" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2636" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2637" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2642" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2643" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2644" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2649" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2650" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2651" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2656" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2657" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2658" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2663" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2664" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2665" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2671" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2952,7 +6584,7 @@
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1083" t="s">
+      <c r="A3" s="2672" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2960,7 +6592,7 @@
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1083" t="s">
+      <c r="A4" s="2672" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -2968,7 +6600,7 @@
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1083" t="s">
+      <c r="A5" s="2672" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -2976,7 +6608,7 @@
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1083" t="s">
+      <c r="A6" s="2672" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -2984,7 +6616,7 @@
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1083" t="s">
+      <c r="A7" s="2672" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -2992,7 +6624,7 @@
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1083" t="s">
+      <c r="A8" s="2672" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -3000,7 +6632,7 @@
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1083" t="s">
+      <c r="A9" s="2672" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3008,7 +6640,7 @@
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1083" t="s">
+      <c r="A10" s="2672" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -3016,7 +6648,7 @@
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1083" t="s">
+      <c r="A11" s="2672" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -3024,7 +6656,7 @@
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1083" t="s">
+      <c r="A12" s="2672" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -3032,7 +6664,7 @@
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1083" t="s">
+      <c r="A13" s="2672" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -3040,7 +6672,7 @@
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1083" t="s">
+      <c r="A14" s="2672" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -3048,7 +6680,7 @@
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1083" t="s">
+      <c r="A15" s="2672" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -3056,7 +6688,7 @@
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1083" t="s">
+      <c r="A16" s="2672" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -3064,7 +6696,7 @@
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
-      <c r="A17" s="1083" t="s">
+      <c r="A17" s="2672" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -3072,7 +6704,7 @@
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="1083" t="s">
+      <c r="A18" s="2672" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -3080,7 +6712,7 @@
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1083" t="s">
+      <c r="A19" s="2672" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -3088,7 +6720,7 @@
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
-      <c r="A20" s="1083" t="s">
+      <c r="A20" s="2672" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -3096,7 +6728,7 @@
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="1083" t="s">
+      <c r="A21" s="2672" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -3104,7 +6736,7 @@
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1083" t="s">
+      <c r="A22" s="2672" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -3323,7 +6955,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="1090" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -3331,7 +6963,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="1090" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -3339,7 +6971,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="1090" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -3347,7 +6979,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="1090" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -3355,7 +6987,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="1090" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -3363,7 +6995,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="1090" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -3371,7 +7003,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="1090" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3379,7 +7011,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="1090" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -3387,7 +7019,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="1090" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -3395,7 +7027,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="1090" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -3403,7 +7035,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="1090" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -3411,7 +7043,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="1090" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -3419,7 +7051,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="1090" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -3427,7 +7059,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="1090" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -3435,7 +7067,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="1090" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -3443,7 +7075,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="1090" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -3451,7 +7083,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="1090" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -3459,7 +7091,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="1090" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -3467,7 +7099,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="1090" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -3475,7 +7107,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="1090" t="s">
         <v>21</v>
       </c>
       <c r="B22">

</xml_diff>